<commit_message>
update several attribute values, add VeryTopConcept
- fixed dct:conbtributor
- changed version property to owl:versionInfo
- updated modified timestamp
- added VeryTopConcept property and links to it
- updated URI to point to github repo version
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graybeal/Documents/git/fair-data-collective/excel2rdf-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{000299B3-E730-FE46-ADFA-D453109265FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCD157E-1BC5-724A-A5FC-60E77C7F7462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="1800" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-terminology" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="111">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -105,9 +105,6 @@
     <t>A definition of NarrowConceptOne, which has a broader concept TopConceptOne.</t>
   </si>
   <si>
-    <t>temp-vocab:TopConceptOne</t>
-  </si>
-  <si>
     <t>This is a template for building a SKOS-based controlled vocabulary. It is used as base of the worflow described in excel2rdf.readthedocs.io/</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>https://purl.org/exampleorg/examplevocab</t>
   </si>
   <si>
     <t>Prefixes for controlled vocabularies, schema and ontologies</t>
@@ -367,9 +361,6 @@
     <t>https://spdx.org/licenses/CC0-1.0</t>
   </si>
   <si>
-    <t>dct:hasVersion^^xsd:string</t>
-  </si>
-  <si>
     <t>dct:created^^xsd:datetime</t>
   </si>
   <si>
@@ -379,15 +370,9 @@
     <t>dct:modified^^xsd:datetime</t>
   </si>
   <si>
-    <t>2022-09-08T00:47:46+00:00</t>
-  </si>
-  <si>
     <t>Example template for building SKOS vocabularies</t>
   </si>
   <si>
-    <t>Title of the vocabulary. These are duplicate so that different systems can all know the title.</t>
-  </si>
-  <si>
     <t>Detailed description of the vocabulary. Saying something about the project, the funder, and the intended application is recommended.</t>
   </si>
   <si>
@@ -499,9 +484,6 @@
     <t>https://orcid.org/0000-0003-2195-3997</t>
   </si>
   <si>
-    <t>dct:conbtributor</t>
-  </si>
-  <si>
     <t>https://orcid.org/0000-0001-8888-635X</t>
   </si>
   <si>
@@ -512,9 +494,6 @@
   </si>
   <si>
     <t>License under which the vocabulary is provided (default is CC0v1.0)</t>
-  </si>
-  <si>
-    <t>0.4.0</t>
   </si>
   <si>
     <t xml:space="preserve">This will be the namespace of the vocabulary—note that it mimics the Main identifier above but includes a '/' at the end so as to join the fragment gracefully.  </t>
@@ -547,6 +526,39 @@
       </rPr>
       <t xml:space="preserve"> is which our base for defining our  SKOS-based controlled vocabulary</t>
     </r>
+  </si>
+  <si>
+    <t>owl:versionInfo</t>
+  </si>
+  <si>
+    <t>0.5.0</t>
+  </si>
+  <si>
+    <t>https://github.com/fair-data-collective/excel2rdf-template/</t>
+  </si>
+  <si>
+    <t>Very Top Concept</t>
+  </si>
+  <si>
+    <t>In this vocabulary this Is a root concept for the whole vocabulary</t>
+  </si>
+  <si>
+    <t>ex-voc:TopConceptOne</t>
+  </si>
+  <si>
+    <t>ex-voc:VeryTopConcept</t>
+  </si>
+  <si>
+    <t>Title of the vocabulary. These are duplicated so that different systems can all know the title.</t>
+  </si>
+  <si>
+    <t>Root Concept</t>
+  </si>
+  <si>
+    <t>dct:contributor</t>
+  </si>
+  <si>
+    <t>2025-05-29T17:18:00-07:00</t>
   </si>
 </sst>
 </file>
@@ -876,7 +888,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -991,6 +1003,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1223,10 +1236,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1254,23 +1267,23 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="10"/>
       <c r="D2" s="32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
@@ -1278,14 +1291,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="13" t="str">
-        <f>B1 &amp; "/"</f>
-        <v>https://purl.org/exampleorg/examplevocab/</v>
+        <v>42</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>102</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -1293,13 +1305,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
@@ -1310,10 +1322,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17">
@@ -1324,10 +1336,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17">
@@ -1335,18 +1347,18 @@
         <v>1</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="31" customHeight="1">
       <c r="A8" s="56" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" s="56"/>
       <c r="C8" s="56"/>
@@ -1357,10 +1369,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16">
@@ -1368,10 +1380,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16">
@@ -1379,22 +1391,22 @@
         <v>6</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16">
       <c r="A12" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="35" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
@@ -1402,10 +1414,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16">
@@ -1413,10 +1425,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16">
@@ -1427,68 +1439,68 @@
         <v>18</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16">
       <c r="A16" s="17" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="16">
       <c r="A17" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="35" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="16">
       <c r="A18" s="17" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="16">
       <c r="A19" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="16">
       <c r="A20" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="31" customHeight="1">
       <c r="A21" s="56" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B21" s="56"/>
       <c r="C21" s="56"/>
@@ -1496,7 +1508,7 @@
     </row>
     <row r="22" spans="1:17" ht="16">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1504,7 +1516,7 @@
     </row>
     <row r="23" spans="1:17" ht="16">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1512,7 +1524,7 @@
     </row>
     <row r="24" spans="1:17" ht="15" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1520,7 +1532,7 @@
     </row>
     <row r="25" spans="1:17" ht="16">
       <c r="A25" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -1528,7 +1540,7 @@
     </row>
     <row r="26" spans="1:17" ht="16">
       <c r="A26" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1541,20 +1553,20 @@
     </row>
     <row r="28" spans="1:17" ht="34" customHeight="1">
       <c r="A28" s="57" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B28" s="58"/>
       <c r="C28" s="58"/>
       <c r="D28" s="59"/>
       <c r="E28" s="53" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F28" s="54"/>
       <c r="G28" s="54"/>
       <c r="H28" s="54"/>
       <c r="I28" s="55"/>
       <c r="J28" s="53" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K28" s="54"/>
       <c r="L28" s="54"/>
@@ -1567,46 +1579,46 @@
     <row r="29" spans="1:17" s="36" customFormat="1" ht="36" customHeight="1">
       <c r="A29" s="11"/>
       <c r="B29" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="I29" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="J29" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="K29" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="F29" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="G29" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="H29" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="I29" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="J29" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="K29" s="36" t="s">
-        <v>93</v>
-      </c>
       <c r="L29" s="36" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="N29" s="36" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="O29" s="36" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="P29" s="36" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="34">
@@ -1629,16 +1641,16 @@
         <v>13</v>
       </c>
       <c r="G30" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="H30" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="I30" s="37" t="s">
-        <v>79</v>
-      </c>
       <c r="J30" s="41" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="K30" s="42" t="s">
         <v>14</v>
@@ -1650,28 +1662,28 @@
         <v>16</v>
       </c>
       <c r="N30" s="41" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="O30" s="41" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P30" s="43" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="16">
       <c r="A31" s="24" t="str">
         <f>IF(ISBLANK($B31),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B31," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>ex-voc:TopConceptOne</v>
+        <v>ex-voc:VeryTopConcept</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="27" t="s">
@@ -1681,60 +1693,64 @@
       <c r="H31" s="27"/>
       <c r="I31" s="49"/>
       <c r="J31" s="50"/>
-      <c r="K31" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="L31" s="51" t="s">
+      <c r="K31" s="60" t="s">
         <v>22</v>
       </c>
+      <c r="L31" s="51"/>
       <c r="M31" s="51"/>
       <c r="N31" s="52"/>
       <c r="O31" s="52"/>
       <c r="P31" s="52"/>
     </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1">
-      <c r="A32" s="23" t="str">
-        <f t="shared" ref="A32:A49" si="0">IF(ISBLANK($B32),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B32," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>ex-voc:NarrowConceptOne</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="46" t="s">
+    <row r="32" spans="1:17" ht="16">
+      <c r="A32" s="24" t="str">
+        <f>IF(ISBLANK($B32),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B32," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ex-voc:TopConceptOne</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="L32" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="45"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="52"/>
+      <c r="O32" s="52"/>
+      <c r="P32" s="52"/>
     </row>
     <row r="33" spans="1:16" ht="15" customHeight="1">
       <c r="A33" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>ex-voc:NarrowConceptTwo</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>32</v>
+        <f t="shared" ref="A33:A50" si="0">IF(ISBLANK($B33),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B33," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ex-voc:NarrowConceptOne</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="29" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="F33" s="30"/>
       <c r="G33" s="30"/>
@@ -1750,89 +1766,89 @@
       <c r="O33" s="45"/>
       <c r="P33" s="45"/>
     </row>
-    <row r="34" spans="1:16" ht="16">
-      <c r="A34" s="24" t="str">
+    <row r="34" spans="1:16" ht="15" customHeight="1">
+      <c r="A34" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>ex-voc:NarrowConceptTwo</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+    </row>
+    <row r="35" spans="1:16" ht="16">
+      <c r="A35" s="24" t="str">
         <f t="shared" si="0"/>
         <v>ex-voc:TopConceptTwo</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="25" t="s">
+      <c r="B35" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27" t="s">
+      <c r="D35" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="51" t="s">
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="L34" s="51" t="s">
+      <c r="L35" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="M34" s="51"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
-    </row>
-    <row r="35" spans="1:16" ht="16">
-      <c r="A35" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>ex-voc:NarrowConceptThree</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="L35" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="M35" s="48"/>
-      <c r="N35" s="45"/>
-      <c r="O35" s="45"/>
-      <c r="P35" s="45"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="52"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="52"/>
     </row>
     <row r="36" spans="1:16" ht="16">
       <c r="A36" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>ex-voc:NarrowConceptFour</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>35</v>
+        <v>ex-voc:NarrowConceptThree</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="38"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="39"/>
       <c r="J36" s="44"/>
       <c r="K36" s="46" t="s">
         <v>18</v>
@@ -1848,20 +1864,30 @@
     <row r="37" spans="1:16" ht="16">
       <c r="A37" s="23" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="39"/>
+        <v>ex-voc:NarrowConceptFour</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="38"/>
       <c r="J37" s="44"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="47"/>
-      <c r="M37" s="47"/>
+      <c r="K37" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="L37" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M37" s="48"/>
       <c r="N37" s="45"/>
       <c r="O37" s="45"/>
       <c r="P37" s="45"/>
@@ -1875,10 +1901,10 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="29"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="38"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="39"/>
       <c r="J38" s="44"/>
       <c r="K38" s="46"/>
       <c r="L38" s="47"/>
@@ -2085,10 +2111,10 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="29"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="40"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="38"/>
       <c r="J48" s="44"/>
       <c r="K48" s="46"/>
       <c r="L48" s="47"/>
@@ -2106,10 +2132,10 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="29"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="38"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="40"/>
       <c r="J49" s="44"/>
       <c r="K49" s="46"/>
       <c r="L49" s="47"/>
@@ -2117,6 +2143,27 @@
       <c r="N49" s="45"/>
       <c r="O49" s="45"/>
       <c r="P49" s="45"/>
+    </row>
+    <row r="50" spans="1:16" ht="16">
+      <c r="A50" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="44"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="47"/>
+      <c r="M50" s="47"/>
+      <c r="N50" s="45"/>
+      <c r="O50" s="45"/>
+      <c r="P50" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2128,17 +2175,18 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" display="http://purl.org/m4m20/subjects/" xr:uid="{E832E347-3333-9047-8EDB-31E925389368}"/>
-    <hyperlink ref="C4" r:id="rId3" display="http://www.w3.org/2004/02/skos/core" xr:uid="{B4111BFB-4FA8-1046-8223-3079DF0BD55D}"/>
-    <hyperlink ref="C5" r:id="rId4" display="http://purl.org/pav/" xr:uid="{5924EF76-29F4-9E45-8A4B-5A411410DCCD}"/>
-    <hyperlink ref="C6" r:id="rId5" display="http://purl.org/dc/terms/" xr:uid="{99E6221A-571B-AB42-9700-1D5B5B026BD5}"/>
-    <hyperlink ref="B17" r:id="rId6" xr:uid="{0371301F-6C79-924A-B126-D11CC3AF0B73}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{CD66A36D-C4EB-8540-B60A-9976CD1112D3}"/>
-    <hyperlink ref="B13" r:id="rId8" xr:uid="{42D7769E-091F-E849-9C69-66BB0B653FB5}"/>
-    <hyperlink ref="B14" r:id="rId9" xr:uid="{B9A99782-37E5-3E49-B675-27FDA25FB7DA}"/>
-    <hyperlink ref="B16" r:id="rId10" xr:uid="{D846468B-1942-3D4E-8273-343712E0C04C}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{F15FDF74-3F86-9043-A674-2372E905C317}"/>
+    <hyperlink ref="B1" r:id="rId1" display="https://purl.org/exampleorg/examplevocab" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" display="http://www.w3.org/2004/02/skos/core" xr:uid="{B4111BFB-4FA8-1046-8223-3079DF0BD55D}"/>
+    <hyperlink ref="C5" r:id="rId3" display="http://purl.org/pav/" xr:uid="{5924EF76-29F4-9E45-8A4B-5A411410DCCD}"/>
+    <hyperlink ref="C6" r:id="rId4" display="http://purl.org/dc/terms/" xr:uid="{99E6221A-571B-AB42-9700-1D5B5B026BD5}"/>
+    <hyperlink ref="B17" r:id="rId5" xr:uid="{0371301F-6C79-924A-B126-D11CC3AF0B73}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{CD66A36D-C4EB-8540-B60A-9976CD1112D3}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{42D7769E-091F-E849-9C69-66BB0B653FB5}"/>
+    <hyperlink ref="B14" r:id="rId8" xr:uid="{B9A99782-37E5-3E49-B675-27FDA25FB7DA}"/>
+    <hyperlink ref="B16" r:id="rId9" xr:uid="{D846468B-1942-3D4E-8273-343712E0C04C}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{F15FDF74-3F86-9043-A674-2372E905C317}"/>
+    <hyperlink ref="C3" r:id="rId11" xr:uid="{F3992104-AE67-F444-980B-146D17F22643}"/>
+    <hyperlink ref="K31" r:id="rId12" xr:uid="{3181E173-0772-E94E-8FEC-8AE411075D3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
fixed prefix bugs, to 0.6.0
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graybeal/Documents/git/fair-data-collective/excel2rdf-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCD157E-1BC5-724A-A5FC-60E77C7F7462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A095E11D-F494-8E4A-B195-D507F9374AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1800" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-terminology" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="110">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t xml:space="preserve">This is yet another top concept which is used to collect a number of narrower concepts. </t>
-  </si>
-  <si>
-    <t>temp-vocab:TopConceptTwo</t>
   </si>
   <si>
     <t>https://orcid.org/0000-0001-6875-5360</t>
@@ -531,9 +528,6 @@
     <t>owl:versionInfo</t>
   </si>
   <si>
-    <t>0.5.0</t>
-  </si>
-  <si>
     <t>https://github.com/fair-data-collective/excel2rdf-template/</t>
   </si>
   <si>
@@ -559,6 +553,9 @@
   </si>
   <si>
     <t>2025-05-29T17:18:00-07:00</t>
+  </si>
+  <si>
+    <t>ex-voc:TopConceptTwo</t>
   </si>
 </sst>
 </file>
@@ -1238,8 +1235,8 @@
   </sheetPr>
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:C21"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1267,23 +1264,23 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="10"/>
       <c r="D2" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
@@ -1291,13 +1288,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -1305,13 +1302,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="D4" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
@@ -1322,10 +1319,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17">
@@ -1336,10 +1333,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17">
@@ -1347,18 +1344,18 @@
         <v>1</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="D7" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="31" customHeight="1">
       <c r="A8" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="56"/>
       <c r="C8" s="56"/>
@@ -1369,10 +1366,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16">
@@ -1380,10 +1377,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16">
@@ -1391,22 +1388,22 @@
         <v>6</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16">
       <c r="A12" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
@@ -1414,10 +1411,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16">
@@ -1425,10 +1422,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16">
@@ -1439,68 +1436,68 @@
         <v>18</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16">
       <c r="A16" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="16">
       <c r="A17" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>50</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>51</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="16">
       <c r="A18" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="B18" s="18">
+        <v>0.6</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="16">
       <c r="A19" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="D19" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="16">
       <c r="A20" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="31" customHeight="1">
       <c r="A21" s="56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="56"/>
       <c r="C21" s="56"/>
@@ -1508,7 +1505,7 @@
     </row>
     <row r="22" spans="1:17" ht="16">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1516,7 +1513,7 @@
     </row>
     <row r="23" spans="1:17" ht="16">
       <c r="A23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1524,7 +1521,7 @@
     </row>
     <row r="24" spans="1:17" ht="15" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1532,7 +1529,7 @@
     </row>
     <row r="25" spans="1:17" ht="16">
       <c r="A25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -1540,7 +1537,7 @@
     </row>
     <row r="26" spans="1:17" ht="16">
       <c r="A26" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1553,20 +1550,20 @@
     </row>
     <row r="28" spans="1:17" ht="34" customHeight="1">
       <c r="A28" s="57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="58"/>
       <c r="C28" s="58"/>
       <c r="D28" s="59"/>
       <c r="E28" s="53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F28" s="54"/>
       <c r="G28" s="54"/>
       <c r="H28" s="54"/>
       <c r="I28" s="55"/>
       <c r="J28" s="53" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K28" s="54"/>
       <c r="L28" s="54"/>
@@ -1579,46 +1576,46 @@
     <row r="29" spans="1:17" s="36" customFormat="1" ht="36" customHeight="1">
       <c r="A29" s="11"/>
       <c r="B29" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>83</v>
-      </c>
       <c r="D29" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E29" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="36" t="s">
+      <c r="G29" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="G29" s="36" t="s">
+      <c r="H29" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="H29" s="36" t="s">
+      <c r="J29" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="I29" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="J29" s="15" t="s">
+      <c r="K29" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="K29" s="36" t="s">
+      <c r="L29" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="N29" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="L29" s="36" t="s">
+      <c r="O29" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="N29" s="36" t="s">
+      <c r="P29" s="36" t="s">
         <v>89</v>
-      </c>
-      <c r="O29" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="P29" s="36" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="34">
@@ -1641,16 +1638,16 @@
         <v>13</v>
       </c>
       <c r="G30" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="J30" s="41" t="s">
         <v>69</v>
-      </c>
-      <c r="H30" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="I30" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="J30" s="41" t="s">
-        <v>70</v>
       </c>
       <c r="K30" s="42" t="s">
         <v>14</v>
@@ -1662,13 +1659,13 @@
         <v>16</v>
       </c>
       <c r="N30" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O30" s="41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P30" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="16">
@@ -1677,13 +1674,13 @@
         <v>ex-voc:VeryTopConcept</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="27" t="s">
@@ -1694,7 +1691,7 @@
       <c r="I31" s="49"/>
       <c r="J31" s="50"/>
       <c r="K31" s="60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L31" s="51"/>
       <c r="M31" s="51"/>
@@ -1708,16 +1705,16 @@
         <v>ex-voc:TopConceptOne</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="25" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F32" s="27" t="s">
         <v>17</v>
@@ -1730,7 +1727,7 @@
         <v>18</v>
       </c>
       <c r="L32" s="51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M32" s="51"/>
       <c r="N32" s="52"/>
@@ -1743,14 +1740,14 @@
         <v>ex-voc:NarrowConceptOne</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F33" s="30"/>
       <c r="G33" s="30"/>
@@ -1758,7 +1755,7 @@
       <c r="I33" s="38"/>
       <c r="J33" s="44"/>
       <c r="K33" s="46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L33" s="47"/>
       <c r="M33" s="47"/>
@@ -1772,14 +1769,14 @@
         <v>ex-voc:NarrowConceptTwo</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F34" s="30"/>
       <c r="G34" s="30"/>
@@ -1787,7 +1784,7 @@
       <c r="I34" s="38"/>
       <c r="J34" s="44"/>
       <c r="K34" s="46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L34" s="47"/>
       <c r="M34" s="47"/>
@@ -1801,16 +1798,16 @@
         <v>ex-voc:TopConceptTwo</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="25" t="s">
         <v>20</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F35" s="27" t="s">
         <v>17</v>
@@ -1823,7 +1820,7 @@
         <v>18</v>
       </c>
       <c r="L35" s="51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M35" s="51"/>
       <c r="N35" s="52"/>
@@ -1836,14 +1833,14 @@
         <v>ex-voc:NarrowConceptThree</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="29" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="F36" s="29"/>
       <c r="G36" s="29"/>
@@ -1854,7 +1851,7 @@
         <v>18</v>
       </c>
       <c r="L36" s="48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M36" s="48"/>
       <c r="N36" s="45"/>
@@ -1867,14 +1864,14 @@
         <v>ex-voc:NarrowConceptFour</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="29" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="F37" s="30"/>
       <c r="G37" s="30"/>
@@ -1885,7 +1882,7 @@
         <v>18</v>
       </c>
       <c r="L37" s="48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M37" s="48"/>
       <c r="N37" s="45"/>
@@ -2175,7 +2172,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="https://purl.org/exampleorg/examplevocab" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C4" r:id="rId2" display="http://www.w3.org/2004/02/skos/core" xr:uid="{B4111BFB-4FA8-1046-8223-3079DF0BD55D}"/>
     <hyperlink ref="C5" r:id="rId3" display="http://purl.org/pav/" xr:uid="{5924EF76-29F4-9E45-8A4B-5A411410DCCD}"/>
     <hyperlink ref="C6" r:id="rId4" display="http://purl.org/dc/terms/" xr:uid="{99E6221A-571B-AB42-9700-1D5B5B026BD5}"/>

</xml_diff>